<commit_message>
Run L-Flange validation with modified code
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/Case-D4600_Tilt-0deg_ShapeFactor1.0.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/Case-D4600_Tilt-0deg_ShapeFactor1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0434D865-7A73-4FA3-8275-DB6DBD03A0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF364C64-5655-4873-A181-45E128FC017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="28680" yWindow="-11130" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5174,13 +5174,34 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5191,27 +5212,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -19349,7 +19349,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -19804,12 +19804,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="173"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19817,12 +19817,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="173"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19830,12 +19830,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="173"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19843,12 +19843,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="172"/>
-      <c r="G8" s="173"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19856,12 +19856,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="173"/>
+      <c r="B9" s="162"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19909,112 +19909,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="163" t="s">
+      <c r="C13" s="165"/>
+      <c r="D13" s="167" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="167"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="164"/>
-      <c r="D14" s="163" t="s">
+      <c r="C14" s="165"/>
+      <c r="D14" s="167" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="167"/>
+      <c r="K14" s="167"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="164"/>
-      <c r="D15" s="163" t="s">
+      <c r="C15" s="165"/>
+      <c r="D15" s="167" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="163"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="167"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="163" t="str">
+      <c r="C16" s="165"/>
+      <c r="D16" s="167" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="163"/>
-      <c r="K16" s="163"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="165" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="164"/>
-      <c r="D17" s="162" t="s">
+      <c r="C17" s="165"/>
+      <c r="D17" s="171" t="s">
         <v>327</v>
       </c>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
+      <c r="J17" s="167"/>
+      <c r="K17" s="167"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="164" t="s">
+      <c r="B18" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="174">
+      <c r="C18" s="165"/>
+      <c r="D18" s="166">
         <v>45432</v>
       </c>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="166"/>
+      <c r="J18" s="166"/>
+      <c r="K18" s="166"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20202,16 +20202,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="173"/>
+      <c r="F28" s="173"/>
+      <c r="G28" s="173"/>
+      <c r="H28" s="173"/>
+      <c r="I28" s="173"/>
+      <c r="J28" s="173"/>
+      <c r="K28" s="174"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24164,6 +24164,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24174,16 +24180,10 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24310,12 +24310,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="173"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24323,12 +24323,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="173"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24336,12 +24336,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="173"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24349,12 +24349,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="172"/>
-      <c r="G8" s="173"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24362,12 +24362,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="173"/>
+      <c r="B9" s="162"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24415,117 +24415,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="163" t="str">
+      <c r="C13" s="165"/>
+      <c r="D13" s="167" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="167"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="164"/>
-      <c r="D14" s="163" t="str">
+      <c r="C14" s="165"/>
+      <c r="D14" s="167" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="167"/>
+      <c r="K14" s="167"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="164"/>
-      <c r="D15" s="163" t="str">
+      <c r="C15" s="165"/>
+      <c r="D15" s="167" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="163"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="167"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="163" t="str">
+      <c r="C16" s="165"/>
+      <c r="D16" s="167" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="163"/>
-      <c r="K16" s="163"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="165" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="164"/>
-      <c r="D17" s="163" t="str">
+      <c r="C17" s="165"/>
+      <c r="D17" s="167" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
+      <c r="J17" s="167"/>
+      <c r="K17" s="167"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="164" t="s">
+      <c r="B18" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="174">
+      <c r="C18" s="165"/>
+      <c r="D18" s="166">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="166"/>
+      <c r="J18" s="166"/>
+      <c r="K18" s="166"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24713,16 +24713,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="173"/>
+      <c r="F28" s="173"/>
+      <c r="G28" s="173"/>
+      <c r="H28" s="173"/>
+      <c r="I28" s="173"/>
+      <c r="J28" s="173"/>
+      <c r="K28" s="174"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28648,13 +28648,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28668,6 +28661,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -28794,12 +28794,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="173"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28807,12 +28807,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="173"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28820,12 +28820,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="173"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28833,12 +28833,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="172"/>
-      <c r="G8" s="173"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28846,12 +28846,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="173"/>
+      <c r="B9" s="162"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28899,117 +28899,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="163" t="str">
+      <c r="C13" s="165"/>
+      <c r="D13" s="167" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="167"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="164"/>
-      <c r="D14" s="163" t="str">
+      <c r="C14" s="165"/>
+      <c r="D14" s="167" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="167"/>
+      <c r="K14" s="167"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="164"/>
-      <c r="D15" s="163" t="str">
+      <c r="C15" s="165"/>
+      <c r="D15" s="167" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="163"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="167"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="163" t="str">
+      <c r="C16" s="165"/>
+      <c r="D16" s="167" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="163"/>
-      <c r="K16" s="163"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="165" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="164"/>
-      <c r="D17" s="163" t="str">
+      <c r="C17" s="165"/>
+      <c r="D17" s="167" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
+      <c r="J17" s="167"/>
+      <c r="K17" s="167"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="164" t="s">
+      <c r="B18" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="174">
+      <c r="C18" s="165"/>
+      <c r="D18" s="166">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="166"/>
+      <c r="J18" s="166"/>
+      <c r="K18" s="166"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29197,16 +29197,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="173"/>
+      <c r="F28" s="173"/>
+      <c r="G28" s="173"/>
+      <c r="H28" s="173"/>
+      <c r="I28" s="173"/>
+      <c r="J28" s="173"/>
+      <c r="K28" s="174"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33132,13 +33132,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33152,6 +33145,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33278,12 +33278,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="171"/>
-      <c r="C5" s="172"/>
-      <c r="D5" s="172"/>
-      <c r="E5" s="172"/>
-      <c r="F5" s="172"/>
-      <c r="G5" s="173"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="163"/>
+      <c r="D5" s="163"/>
+      <c r="E5" s="163"/>
+      <c r="F5" s="163"/>
+      <c r="G5" s="164"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33291,12 +33291,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="172"/>
-      <c r="D6" s="172"/>
-      <c r="E6" s="172"/>
-      <c r="F6" s="172"/>
-      <c r="G6" s="173"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="163"/>
+      <c r="D6" s="163"/>
+      <c r="E6" s="163"/>
+      <c r="F6" s="163"/>
+      <c r="G6" s="164"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33304,12 +33304,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="171"/>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172"/>
-      <c r="E7" s="172"/>
-      <c r="F7" s="172"/>
-      <c r="G7" s="173"/>
+      <c r="B7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33317,12 +33317,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="171"/>
-      <c r="C8" s="172"/>
-      <c r="D8" s="172"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="172"/>
-      <c r="G8" s="173"/>
+      <c r="B8" s="162"/>
+      <c r="C8" s="163"/>
+      <c r="D8" s="163"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="163"/>
+      <c r="G8" s="164"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33330,12 +33330,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="171"/>
-      <c r="C9" s="172"/>
-      <c r="D9" s="172"/>
-      <c r="E9" s="172"/>
-      <c r="F9" s="172"/>
-      <c r="G9" s="173"/>
+      <c r="B9" s="162"/>
+      <c r="C9" s="163"/>
+      <c r="D9" s="163"/>
+      <c r="E9" s="163"/>
+      <c r="F9" s="163"/>
+      <c r="G9" s="164"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33383,117 +33383,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="165" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="164"/>
-      <c r="D13" s="163" t="str">
+      <c r="C13" s="165"/>
+      <c r="D13" s="167" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="163"/>
-      <c r="F13" s="163"/>
-      <c r="G13" s="163"/>
-      <c r="H13" s="163"/>
-      <c r="I13" s="163"/>
-      <c r="J13" s="163"/>
-      <c r="K13" s="163"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="167"/>
+      <c r="G13" s="167"/>
+      <c r="H13" s="167"/>
+      <c r="I13" s="167"/>
+      <c r="J13" s="167"/>
+      <c r="K13" s="167"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="164" t="s">
+      <c r="B14" s="165" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="164"/>
-      <c r="D14" s="163" t="str">
+      <c r="C14" s="165"/>
+      <c r="D14" s="167" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="163"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="163"/>
-      <c r="J14" s="163"/>
-      <c r="K14" s="163"/>
+      <c r="E14" s="167"/>
+      <c r="F14" s="167"/>
+      <c r="G14" s="167"/>
+      <c r="H14" s="167"/>
+      <c r="I14" s="167"/>
+      <c r="J14" s="167"/>
+      <c r="K14" s="167"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="164" t="s">
+      <c r="B15" s="165" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="164"/>
-      <c r="D15" s="163" t="str">
+      <c r="C15" s="165"/>
+      <c r="D15" s="167" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="163"/>
-      <c r="F15" s="163"/>
-      <c r="G15" s="163"/>
-      <c r="H15" s="163"/>
-      <c r="I15" s="163"/>
-      <c r="J15" s="163"/>
-      <c r="K15" s="163"/>
+      <c r="E15" s="167"/>
+      <c r="F15" s="167"/>
+      <c r="G15" s="167"/>
+      <c r="H15" s="167"/>
+      <c r="I15" s="167"/>
+      <c r="J15" s="167"/>
+      <c r="K15" s="167"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="164" t="s">
+      <c r="B16" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="164"/>
-      <c r="D16" s="163" t="str">
+      <c r="C16" s="165"/>
+      <c r="D16" s="167" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="163"/>
-      <c r="F16" s="163"/>
-      <c r="G16" s="163"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="163"/>
-      <c r="J16" s="163"/>
-      <c r="K16" s="163"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="167"/>
+      <c r="G16" s="167"/>
+      <c r="H16" s="167"/>
+      <c r="I16" s="167"/>
+      <c r="J16" s="167"/>
+      <c r="K16" s="167"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="164" t="s">
+      <c r="B17" s="165" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="164"/>
-      <c r="D17" s="163" t="str">
+      <c r="C17" s="165"/>
+      <c r="D17" s="167" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="163"/>
-      <c r="F17" s="163"/>
-      <c r="G17" s="163"/>
-      <c r="H17" s="163"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="163"/>
+      <c r="E17" s="167"/>
+      <c r="F17" s="167"/>
+      <c r="G17" s="167"/>
+      <c r="H17" s="167"/>
+      <c r="I17" s="167"/>
+      <c r="J17" s="167"/>
+      <c r="K17" s="167"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="164" t="s">
+      <c r="B18" s="165" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="164"/>
-      <c r="D18" s="174">
+      <c r="C18" s="165"/>
+      <c r="D18" s="166">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
+      <c r="E18" s="166"/>
+      <c r="F18" s="166"/>
+      <c r="G18" s="166"/>
+      <c r="H18" s="166"/>
+      <c r="I18" s="166"/>
+      <c r="J18" s="166"/>
+      <c r="K18" s="166"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33681,16 +33681,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="173"/>
+      <c r="D28" s="173"/>
+      <c r="E28" s="173"/>
+      <c r="F28" s="173"/>
+      <c r="G28" s="173"/>
+      <c r="H28" s="173"/>
+      <c r="I28" s="173"/>
+      <c r="J28" s="173"/>
+      <c r="K28" s="174"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37616,13 +37616,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37636,6 +37629,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -37672,7 +37672,7 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -42525,6 +42525,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -42777,24 +42794,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42811,29 +42836,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fatigue: added unit test; fixed minor bugs
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/Case-D4600_Tilt-0deg_ShapeFactor1.0.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/Case-D4600_Tilt-0deg_ShapeFactor1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF364C64-5655-4873-A181-45E128FC017B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85129047-D411-48A8-9CE1-0D047721263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-11130" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-22245" yWindow="5970" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5174,6 +5174,24 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5192,26 +5210,8 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -19763,32 +19763,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -19804,12 +19804,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -19817,12 +19817,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -19830,12 +19830,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -19843,12 +19843,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -19856,12 +19856,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -19909,112 +19909,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="s">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="s">
         <v>102</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="s">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="s">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="171" t="s">
+      <c r="C17" s="171"/>
+      <c r="D17" s="174" t="s">
         <v>327</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20202,16 +20202,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24164,6 +24164,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -24180,10 +24184,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24269,32 +24269,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -24310,12 +24310,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24323,12 +24323,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24336,12 +24336,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24349,12 +24349,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24362,12 +24362,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24415,117 +24415,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -24713,16 +24713,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -28648,6 +28648,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -28661,13 +28668,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -28753,32 +28753,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -28794,12 +28794,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -28807,12 +28807,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -28820,12 +28820,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -28833,12 +28833,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -28846,12 +28846,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -28899,117 +28899,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29197,16 +29197,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33132,6 +33132,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33145,13 +33152,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33237,32 +33237,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="168" t="s">
+      <c r="A3" s="165" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="169"/>
-      <c r="C3" s="169"/>
-      <c r="D3" s="169"/>
-      <c r="E3" s="169"/>
-      <c r="F3" s="169"/>
-      <c r="G3" s="169"/>
-      <c r="H3" s="169"/>
-      <c r="I3" s="169"/>
-      <c r="J3" s="169"/>
-      <c r="K3" s="169"/>
+      <c r="B3" s="166"/>
+      <c r="C3" s="166"/>
+      <c r="D3" s="166"/>
+      <c r="E3" s="166"/>
+      <c r="F3" s="166"/>
+      <c r="G3" s="166"/>
+      <c r="H3" s="166"/>
+      <c r="I3" s="166"/>
+      <c r="J3" s="166"/>
+      <c r="K3" s="166"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="170" t="s">
+      <c r="B4" s="167" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="170"/>
-      <c r="D4" s="170"/>
-      <c r="E4" s="170"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
+      <c r="C4" s="167"/>
+      <c r="D4" s="167"/>
+      <c r="E4" s="167"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
       <c r="H4" s="47" t="s">
         <v>14</v>
       </c>
@@ -33278,12 +33278,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="168"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="170"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33291,12 +33291,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="168"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="169"/>
+      <c r="F6" s="169"/>
+      <c r="G6" s="170"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33304,12 +33304,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33317,12 +33317,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="168"/>
+      <c r="C8" s="169"/>
+      <c r="D8" s="169"/>
+      <c r="E8" s="169"/>
+      <c r="F8" s="169"/>
+      <c r="G8" s="170"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33330,12 +33330,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="169"/>
+      <c r="E9" s="169"/>
+      <c r="F9" s="169"/>
+      <c r="G9" s="170"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33383,117 +33383,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="165" t="s">
+      <c r="B13" s="171" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="165"/>
-      <c r="D13" s="167" t="str">
+      <c r="C13" s="171"/>
+      <c r="D13" s="173" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="167"/>
-      <c r="F13" s="167"/>
-      <c r="G13" s="167"/>
-      <c r="H13" s="167"/>
-      <c r="I13" s="167"/>
-      <c r="J13" s="167"/>
-      <c r="K13" s="167"/>
+      <c r="E13" s="173"/>
+      <c r="F13" s="173"/>
+      <c r="G13" s="173"/>
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="173"/>
+      <c r="K13" s="173"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="165" t="s">
+      <c r="B14" s="171" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="165"/>
-      <c r="D14" s="167" t="str">
+      <c r="C14" s="171"/>
+      <c r="D14" s="173" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="167"/>
-      <c r="F14" s="167"/>
-      <c r="G14" s="167"/>
-      <c r="H14" s="167"/>
-      <c r="I14" s="167"/>
-      <c r="J14" s="167"/>
-      <c r="K14" s="167"/>
+      <c r="E14" s="173"/>
+      <c r="F14" s="173"/>
+      <c r="G14" s="173"/>
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="173"/>
+      <c r="K14" s="173"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="165" t="s">
+      <c r="B15" s="171" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="165"/>
-      <c r="D15" s="167" t="str">
+      <c r="C15" s="171"/>
+      <c r="D15" s="173" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="167"/>
-      <c r="F15" s="167"/>
-      <c r="G15" s="167"/>
-      <c r="H15" s="167"/>
-      <c r="I15" s="167"/>
-      <c r="J15" s="167"/>
-      <c r="K15" s="167"/>
+      <c r="E15" s="173"/>
+      <c r="F15" s="173"/>
+      <c r="G15" s="173"/>
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="173"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="171" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="165"/>
-      <c r="D16" s="167" t="str">
+      <c r="C16" s="171"/>
+      <c r="D16" s="173" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="167"/>
-      <c r="F16" s="167"/>
-      <c r="G16" s="167"/>
-      <c r="H16" s="167"/>
-      <c r="I16" s="167"/>
-      <c r="J16" s="167"/>
-      <c r="K16" s="167"/>
+      <c r="E16" s="173"/>
+      <c r="F16" s="173"/>
+      <c r="G16" s="173"/>
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="173"/>
+      <c r="K16" s="173"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="165" t="s">
+      <c r="B17" s="171" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="165"/>
-      <c r="D17" s="167" t="str">
+      <c r="C17" s="171"/>
+      <c r="D17" s="173" t="str">
         <f>Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="167"/>
-      <c r="G17" s="167"/>
-      <c r="H17" s="167"/>
-      <c r="I17" s="167"/>
-      <c r="J17" s="167"/>
-      <c r="K17" s="167"/>
+      <c r="E17" s="173"/>
+      <c r="F17" s="173"/>
+      <c r="G17" s="173"/>
+      <c r="H17" s="173"/>
+      <c r="I17" s="173"/>
+      <c r="J17" s="173"/>
+      <c r="K17" s="173"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="165" t="s">
+      <c r="B18" s="171" t="s">
         <v>96</v>
       </c>
-      <c r="C18" s="165"/>
-      <c r="D18" s="166">
+      <c r="C18" s="171"/>
+      <c r="D18" s="172">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="166"/>
-      <c r="F18" s="166"/>
-      <c r="G18" s="166"/>
-      <c r="H18" s="166"/>
-      <c r="I18" s="166"/>
-      <c r="J18" s="166"/>
-      <c r="K18" s="166"/>
+      <c r="E18" s="172"/>
+      <c r="F18" s="172"/>
+      <c r="G18" s="172"/>
+      <c r="H18" s="172"/>
+      <c r="I18" s="172"/>
+      <c r="J18" s="172"/>
+      <c r="K18" s="172"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -33681,16 +33681,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173"/>
-      <c r="D28" s="173"/>
-      <c r="E28" s="173"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="173"/>
-      <c r="H28" s="173"/>
-      <c r="I28" s="173"/>
-      <c r="J28" s="173"/>
-      <c r="K28" s="174"/>
+      <c r="B28" s="162"/>
+      <c r="C28" s="163"/>
+      <c r="D28" s="163"/>
+      <c r="E28" s="163"/>
+      <c r="F28" s="163"/>
+      <c r="G28" s="163"/>
+      <c r="H28" s="163"/>
+      <c r="I28" s="163"/>
+      <c r="J28" s="163"/>
+      <c r="K28" s="164"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -37616,6 +37616,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -37629,13 +37636,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -37672,8 +37672,8 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="A1:X135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -42525,23 +42525,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -42794,32 +42777,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42836,4 +42811,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>